<commit_message>
I made GUI input for SSC
</commit_message>
<xml_diff>
--- a/Variable_SSC.xlsx
+++ b/Variable_SSC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william_hess/Desktop/FSAE/taiyangie-LinkageForceAnalyzer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F2295EC-3E5C-554A-A7FA-F9688844C421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9B9942-9D43-FD4A-976E-B09E94840EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="17300" windowHeight="17440" xr2:uid="{BC6CD8CD-A3D1-9D46-89DC-0B65502A9D27}"/>
+    <workbookView xWindow="320" yWindow="500" windowWidth="17300" windowHeight="17440" xr2:uid="{BC6CD8CD-A3D1-9D46-89DC-0B65502A9D27}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>Turn Radius</t>
   </si>
   <si>
-    <t>R</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
@@ -86,13 +83,16 @@
     <t>Rear Roll Rate</t>
   </si>
   <si>
-    <t>K_thetaf</t>
-  </si>
-  <si>
-    <t>K_thetar</t>
-  </si>
-  <si>
     <t>in-lb/deg</t>
+  </si>
+  <si>
+    <t>T_rad</t>
+  </si>
+  <si>
+    <t>K_f</t>
+  </si>
+  <si>
+    <t>K_r</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,54 +491,54 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>